<commit_message>
matching references to students
</commit_message>
<xml_diff>
--- a/dummy_references_responses_data.xlsx
+++ b/dummy_references_responses_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
   <si>
     <t>Email Address</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Student Last Name</t>
   </si>
   <si>
+    <t>Letter</t>
+  </si>
+  <si>
     <t>reference1@gmail.com</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>Ukunze Dukorerimana</t>
+  </si>
+  <si>
+    <t>PDF</t>
   </si>
   <si>
     <t>reference2@gmail.com</t>
@@ -531,383 +537,467 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>